<commit_message>
Issue 6447 - Testing Judge Algo
</commit_message>
<xml_diff>
--- a/spec/support/twoInJulyJudgeSpreadsheet.xlsx
+++ b/spec/support/twoInJulyJudgeSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarramirez/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1503253D-1487-5345-A311-721FA2226552}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9D56AE-86CC-4549-9FC2-22A4D4D3095A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31960" yWindow="2920" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,12 +447,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,6 +455,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1670,12 +1670,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1791,7 +1791,7 @@
       <c r="B8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="33" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="28">
@@ -1808,10 +1808,10 @@
       <c r="B9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="34">
         <v>861</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="35" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="31"/>

</xml_diff>